<commit_message>
TMTI0112743_VerifyConclusionDateDoNotAppearOnTheExistingCFLOBEngagements - Final - 5th Aug 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTI0112743_VerifyConclusionDateDoNotAppearOnTheExistingCFLOBEngagements.xlsx
+++ b/TestData/TMTI0112743_VerifyConclusionDateDoNotAppearOnTheExistingCFLOBEngagements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECAFE29-CDEF-40B6-A05B-05E7453F6A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4561903B-852A-4328-9635-2833FE24E78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Dea Team Member</t>
   </si>
@@ -49,6 +49,30 @@
   </si>
   <si>
     <t>Project Racer - Dual Track</t>
+  </si>
+  <si>
+    <t>EngagementLOB</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>Salem Harbor</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Spencer Anderson</t>
+  </si>
+  <si>
+    <t>Karan Chopra</t>
+  </si>
+  <si>
+    <t>FVA</t>
+  </si>
+  <si>
+    <t>Arista Networks - Big Switch PPA</t>
   </si>
 </sst>
 </file>
@@ -375,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,6 +420,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -404,25 +438,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>